<commit_message>
3 estimate given to nuwa mam
</commit_message>
<xml_diff>
--- a/ofc/estimates/estimates/चनौटे, घट्टेखोला सडक/V.xlsx
+++ b/ofc/estimates/estimates/चनौटे, घट्टेखोला सडक/V.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="local" sheetId="19" r:id="rId1"/>
@@ -429,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -508,9 +508,6 @@
     </xf>
     <xf numFmtId="1" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -570,12 +567,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -583,16 +595,26 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -610,31 +632,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1318,8 +1315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q80"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1337,113 +1334,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1494,8 +1491,8 @@
       <c r="G9" s="23"/>
       <c r="H9" s="22"/>
       <c r="I9" s="23"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="58"/>
+      <c r="J9" s="39"/>
+      <c r="K9" s="57"/>
       <c r="M9">
         <f>13500*10</f>
         <v>135000</v>
@@ -1507,30 +1504,30 @@
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="35">
+      <c r="C10" s="34">
         <v>1</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="36">
         <v>90</v>
       </c>
-      <c r="E10" s="37">
+      <c r="E10" s="36">
         <f>10/3.281</f>
         <v>3.047851264858275</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="36">
         <v>0.125</v>
       </c>
-      <c r="G10" s="38">
+      <c r="G10" s="37">
         <f>PRODUCT(C10:F10)</f>
         <v>34.288326729655594</v>
       </c>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="58"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="57"/>
       <c r="M10" t="s">
         <v>45</v>
       </c>
@@ -1543,7 +1540,7 @@
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="19"/>
@@ -1560,11 +1557,11 @@
       <c r="I11" s="23">
         <v>1693.85</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="39">
         <f>G11*I11</f>
         <v>58079.282231027122</v>
       </c>
-      <c r="K11" s="58"/>
+      <c r="K11" s="57"/>
       <c r="M11">
         <f>3244.12</f>
         <v>3244.12</v>
@@ -1583,7 +1580,7 @@
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="19"/>
@@ -1593,7 +1590,7 @@
       <c r="G12" s="23"/>
       <c r="H12" s="22"/>
       <c r="I12" s="23"/>
-      <c r="J12" s="40">
+      <c r="J12" s="39">
         <f>0.13*G11*446551.8/300</f>
         <v>6634.989408716855</v>
       </c>
@@ -1609,7 +1606,7 @@
       <c r="G13" s="23"/>
       <c r="H13" s="22"/>
       <c r="I13" s="23"/>
-      <c r="J13" s="40"/>
+      <c r="J13" s="39"/>
       <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1625,7 +1622,7 @@
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
       <c r="F14" s="21"/>
-      <c r="G14" s="33">
+      <c r="G14" s="32">
         <f t="shared" ref="G14" si="0">PRODUCT(C14:F14)</f>
         <v>1</v>
       </c>
@@ -1635,7 +1632,7 @@
       <c r="I14" s="23">
         <v>500</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="32">
         <f>G14*I14</f>
         <v>500</v>
       </c>
@@ -1651,230 +1648,235 @@
       <c r="G15" s="23"/>
       <c r="H15" s="22"/>
       <c r="I15" s="23"/>
-      <c r="J15" s="40"/>
+      <c r="J15" s="39"/>
       <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="41" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40">
+      <c r="C16" s="41"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39">
         <f>SUM(J9:J14)</f>
         <v>65214.27163974398</v>
       </c>
-      <c r="K16" s="35"/>
+      <c r="K16" s="34"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="56"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="52"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
+      <c r="K17" s="51"/>
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
+      <c r="A18" s="44"/>
       <c r="B18" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="60">
+      <c r="C18" s="61">
         <f>J16</f>
         <v>65214.27163974398</v>
       </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="38">
+      <c r="D18" s="61"/>
+      <c r="E18" s="37">
         <v>100</v>
       </c>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="49"/>
-      <c r="K18" s="50"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="49"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="81">
+      <c r="C19" s="62">
         <v>50000</v>
       </c>
-      <c r="D19" s="81"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="44"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="42"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="50"/>
       <c r="B20" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C20" s="81">
+      <c r="C20" s="62">
         <f>C19-C22-C23</f>
         <v>47500</v>
       </c>
-      <c r="D20" s="81"/>
-      <c r="E20" s="38">
+      <c r="D20" s="62"/>
+      <c r="E20" s="37">
         <f>C20/C18*100</f>
         <v>72.836817472100307</v>
       </c>
-      <c r="F20" s="44"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="44"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="43"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
+      <c r="A21" s="50"/>
       <c r="B21" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="60">
+      <c r="C21" s="61">
         <f>C18-C20</f>
         <v>17714.27163974398</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="38">
+      <c r="D21" s="61"/>
+      <c r="E21" s="37">
         <f>100-E20</f>
         <v>27.163182527899693</v>
       </c>
-      <c r="F21" s="44"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="44"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="43"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="51"/>
+      <c r="A22" s="50"/>
       <c r="B22" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="60">
+      <c r="C22" s="61">
         <f>C19*0.03</f>
         <v>1500</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="38">
+      <c r="D22" s="61"/>
+      <c r="E22" s="37">
         <v>3</v>
       </c>
-      <c r="F22" s="44"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="44"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="43"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="60">
+      <c r="C23" s="61">
         <f>C19*0.02</f>
         <v>1000</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="38">
+      <c r="D23" s="61"/>
+      <c r="E23" s="37">
         <v>2</v>
       </c>
-      <c r="F23" s="44"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="44"/>
-    </row>
-    <row r="24" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="52"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="52"/>
-      <c r="K24" s="52"/>
-    </row>
-    <row r="25" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="43"/>
+    </row>
+    <row r="24" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="51"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
+      <c r="G24" s="51"/>
+      <c r="H24" s="51"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="51"/>
+    </row>
+    <row r="25" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="A7:F7"/>
     <mergeCell ref="H7:K7"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="C19:D19"/>
@@ -1885,11 +1887,6 @@
     <mergeCell ref="A5:K5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -1906,8 +1903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1926,90 +1923,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="80"/>
+      <c r="F2" s="80"/>
+      <c r="G2" s="80"/>
+      <c r="H2" s="80"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
+      <c r="K2" s="80"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="81" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
+      <c r="E5" s="81"/>
+      <c r="F5" s="81"/>
+      <c r="G5" s="81"/>
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="81"/>
+      <c r="K5" s="81"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="69" t="e">
+      <c r="C6" s="77">
         <f>F18</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D6" s="70"/>
+        <v>65214.27163974398</v>
+      </c>
+      <c r="D6" s="78"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -2017,11 +2014,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="69" t="e">
+      <c r="J6" s="77">
         <f>I18</f>
-        <v>#REF!</v>
-      </c>
-      <c r="K6" s="70"/>
+        <v>52552.022063940392</v>
+      </c>
+      <c r="K6" s="78"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
@@ -2030,77 +2027,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="I7" s="77" t="s">
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="I7" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="e">
+      <c r="A8" s="67" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="I8" s="78" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="I8" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="e">
+      <c r="A9" s="75" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="I9" s="78" t="s">
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="I9" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80" t="s">
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="74" t="s">
+      <c r="H11" s="76"/>
+      <c r="I11" s="76"/>
+      <c r="J11" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="71" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="70"/>
+      <c r="C12" s="70"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -2119,77 +2116,80 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="75"/>
+      <c r="J12" s="70"/>
+      <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B13" s="31" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C13" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D13" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E13" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F13" s="12" t="e">
+      <c r="A13" s="26">
+        <f>local!A9</f>
+        <v>1</v>
+      </c>
+      <c r="B13" s="31" t="str">
+        <f>local!B9</f>
+        <v>Providing and laying  local/ washing sub-base   on prepared surface, mixing  at OMC, and compacting  to achieve the desired density, complete as per Drawing and Technical Specifications., By Mechanical means</v>
+      </c>
+      <c r="C13" s="12" t="str">
+        <f>local!H11</f>
+        <v>m3</v>
+      </c>
+      <c r="D13" s="12">
+        <f>local!G11</f>
+        <v>34.288326729655594</v>
+      </c>
+      <c r="E13" s="12">
+        <f>local!I11</f>
+        <v>1693.85</v>
+      </c>
+      <c r="F13" s="12">
         <f>D13*E13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G13" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H13" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I13" s="12" t="e">
+        <v>58079.282231027122</v>
+      </c>
+      <c r="G13" s="12">
+        <f>V!G24</f>
+        <v>27.844258417424825</v>
+      </c>
+      <c r="H13" s="12">
+        <f>V!I24</f>
+        <v>1693.85</v>
+      </c>
+      <c r="I13" s="12">
         <f>G13*H13</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J13" s="27" t="e">
+        <v>47163.997120355038</v>
+      </c>
+      <c r="J13" s="27">
         <f>I13-F13</f>
-        <v>#REF!</v>
+        <v>-10915.285110672085</v>
       </c>
       <c r="K13" s="14"/>
     </row>
     <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
-      <c r="B14" s="32" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="B14" s="31" t="str">
+        <f>local!B12</f>
+        <v>-VAT 13% calculation</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
-      <c r="F14" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
+      <c r="F14" s="12">
+        <f>local!J12</f>
+        <v>6634.989408716855</v>
       </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
-      <c r="I14" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J14" s="27"/>
+      <c r="I14" s="12">
+        <f>V!J25</f>
+        <v>5388.0249435853566</v>
+      </c>
+      <c r="J14" s="27">
+        <f>I14-F14</f>
+        <v>-1246.9644651314984</v>
+      </c>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="28"/>
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="26"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="12"/>
@@ -2201,45 +2201,45 @@
       <c r="K15" s="14"/>
     </row>
     <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="B16" s="30" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C16" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="D16" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="E16" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="F16" s="12" t="e">
+      <c r="A16" s="26">
+        <f>local!A14</f>
+        <v>2</v>
+      </c>
+      <c r="B16" s="30" t="str">
+        <f>local!B14</f>
+        <v>Information board (सुचना पाटि)</v>
+      </c>
+      <c r="C16" s="12" t="str">
+        <f>local!H14</f>
+        <v>no.</v>
+      </c>
+      <c r="D16" s="12">
+        <f>local!G14</f>
+        <v>1</v>
+      </c>
+      <c r="E16" s="12">
+        <f>local!I14</f>
+        <v>500</v>
+      </c>
+      <c r="F16" s="12">
         <f>D16*E16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="G16" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="H16" s="12" t="e">
-        <f>#REF!</f>
-        <v>#REF!</v>
-      </c>
-      <c r="I16" s="12" t="e">
+        <v>500</v>
+      </c>
+      <c r="G16" s="12">
+        <f>V!G27</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="12">
+        <f>V!I27</f>
+        <v>500</v>
+      </c>
+      <c r="I16" s="12">
         <f>G16*H16</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J16" s="27" t="e">
+        <v>0</v>
+      </c>
+      <c r="J16" s="27">
         <f>I16-F16</f>
-        <v>#REF!</v>
+        <v>-500</v>
       </c>
       <c r="K16" s="14"/>
     </row>
@@ -2264,24 +2264,31 @@
       <c r="C18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-      <c r="F18" s="7" t="e">
+      <c r="F18" s="7">
         <f>SUM(F13:F16)</f>
-        <v>#REF!</v>
+        <v>65214.27163974398</v>
       </c>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="7" t="e">
+      <c r="I18" s="7">
         <f>SUM(I13:I16)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="J18" s="13" t="e">
+        <v>52552.022063940392</v>
+      </c>
+      <c r="J18" s="13">
         <f>I18-F18</f>
-        <v>#REF!</v>
+        <v>-12662.249575803588</v>
       </c>
       <c r="K18" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -2295,13 +2302,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2319,8 +2319,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O23" sqref="O23"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,113 +2339,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
+      <c r="B1" s="63"/>
+      <c r="C1" s="63"/>
+      <c r="D1" s="63"/>
+      <c r="E1" s="63"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="63"/>
+      <c r="H1" s="63"/>
+      <c r="I1" s="63"/>
+      <c r="J1" s="63"/>
+      <c r="K1" s="63"/>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
     </row>
     <row r="4" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="67" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="62" t="s">
+      <c r="H7" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
     </row>
     <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -2496,560 +2496,560 @@
       <c r="G9" s="23"/>
       <c r="H9" s="22"/>
       <c r="I9" s="23"/>
-      <c r="J9" s="40"/>
-      <c r="K9" s="58"/>
-      <c r="N9" s="59" t="s">
+      <c r="J9" s="39"/>
+      <c r="K9" s="57"/>
+      <c r="N9" s="58" t="s">
         <v>64</v>
       </c>
-      <c r="O9" s="59" t="s">
+      <c r="O9" s="58" t="s">
         <v>63</v>
       </c>
-      <c r="P9" s="59" t="s">
+      <c r="P9" s="58" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="58"/>
-      <c r="O10" s="82">
+      <c r="C10" s="34"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="57"/>
+      <c r="O10" s="59">
         <f>8.75/3.281</f>
         <v>2.6668698567509903</v>
       </c>
-      <c r="P10" s="82">
+      <c r="P10" s="59">
         <f>0.42/3.281</f>
         <v>0.12800975312404753</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="34">
         <v>1</v>
       </c>
-      <c r="D11" s="37">
+      <c r="D11" s="36">
         <f>N11</f>
         <v>5</v>
       </c>
-      <c r="E11" s="37">
+      <c r="E11" s="36">
         <f>(O10+O11)/2</f>
         <v>2.7049679975617189</v>
       </c>
-      <c r="F11" s="37">
+      <c r="F11" s="36">
         <f>(P10+P11)/2</f>
         <v>0.12800975312404753</v>
       </c>
-      <c r="G11" s="38">
+      <c r="G11" s="37">
         <f>PRODUCT(C11:F11)</f>
         <v>1.7313114278816242</v>
       </c>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="58"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="57"/>
       <c r="N11">
         <v>5</v>
       </c>
-      <c r="O11" s="82">
+      <c r="O11" s="59">
         <f>9/3.281</f>
         <v>2.7430661383724475</v>
       </c>
-      <c r="P11" s="82">
+      <c r="P11" s="59">
         <f>0.42/3.281</f>
         <v>0.12800975312404753</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <v>1</v>
       </c>
-      <c r="D12" s="37">
+      <c r="D12" s="36">
         <f t="shared" ref="D12:D22" si="0">N12</f>
         <v>5</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="36">
         <f t="shared" ref="E12:E23" si="1">(O11+O12)/2</f>
         <v>3.047851264858275</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="36">
         <f t="shared" ref="F12:F23" si="2">(P11+P12)/2</f>
         <v>0.14020115818348061</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="37">
         <f t="shared" ref="G12:G22" si="3">PRODUCT(C12:F12)</f>
         <v>2.1365613865205826</v>
       </c>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="58"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="57"/>
       <c r="N12">
         <v>5</v>
       </c>
-      <c r="O12" s="82">
+      <c r="O12" s="59">
         <f>11/3.281</f>
         <v>3.3526363913441024</v>
       </c>
-      <c r="P12" s="82">
+      <c r="P12" s="59">
         <f>0.5/3.281</f>
         <v>0.15239256324291373</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="34">
         <v>1</v>
       </c>
-      <c r="D13" s="37">
+      <c r="D13" s="36">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E13" s="37">
+      <c r="E13" s="36">
         <f t="shared" si="1"/>
         <v>3.1341306956720514</v>
       </c>
-      <c r="F13" s="37">
+      <c r="F13" s="36">
+        <f t="shared" si="2"/>
+        <v>0.14020115818348061</v>
+      </c>
+      <c r="G13" s="37">
+        <f t="shared" si="3"/>
+        <v>2.1970437671580973</v>
+      </c>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="57"/>
+      <c r="N13">
+        <v>5</v>
+      </c>
+      <c r="O13" s="59">
+        <f>9.33/3.2/1</f>
+        <v>2.9156249999999999</v>
+      </c>
+      <c r="P13" s="59">
+        <f>0.42/3.281</f>
+        <v>0.12800975312404753</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+      <c r="B14" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="34">
+        <v>1</v>
+      </c>
+      <c r="D14" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E14" s="36">
+        <f t="shared" si="1"/>
+        <v>2.9055418508076807</v>
+      </c>
+      <c r="F14" s="36">
+        <f t="shared" si="2"/>
+        <v>0.14020115818348061</v>
+      </c>
+      <c r="G14" s="37">
+        <f t="shared" si="3"/>
+        <v>2.0368016631690531</v>
+      </c>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="57"/>
+      <c r="N14">
+        <v>5</v>
+      </c>
+      <c r="O14" s="59">
+        <f>9.5/3.281</f>
+        <v>2.895458701615361</v>
+      </c>
+      <c r="P14" s="59">
+        <f>0.5/3.281</f>
+        <v>0.15239256324291373</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="34">
+        <v>1</v>
+      </c>
+      <c r="D15" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E15" s="36">
+        <f t="shared" si="1"/>
+        <v>2.8192624199939043</v>
+      </c>
+      <c r="F15" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="G15" s="37">
+        <f t="shared" si="3"/>
+        <v>2.1144468149954281</v>
+      </c>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="57"/>
+      <c r="N15">
+        <v>5</v>
+      </c>
+      <c r="O15" s="59">
+        <f>9/3.281</f>
+        <v>2.7430661383724475</v>
+      </c>
+      <c r="P15" s="59">
+        <f>0.583/3.281</f>
+        <v>0.1776897287412374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+      <c r="B16" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="34">
+        <v>1</v>
+      </c>
+      <c r="D16" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E16" s="36">
+        <f t="shared" si="1"/>
+        <v>2.6668698567509903</v>
+      </c>
+      <c r="F16" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="G16" s="37">
+        <f t="shared" si="3"/>
+        <v>2.0001523925632427</v>
+      </c>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+      <c r="K16" s="57"/>
+      <c r="N16">
+        <v>5</v>
+      </c>
+      <c r="O16" s="59">
+        <f>8.5/3.281</f>
+        <v>2.5906735751295336</v>
+      </c>
+      <c r="P16" s="59">
+        <f>0.75/3.281</f>
+        <v>0.22858884486437062</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+      <c r="B17" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="34">
+        <v>1</v>
+      </c>
+      <c r="D17" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E17" s="36">
+        <f t="shared" si="1"/>
+        <v>2.5906735751295336</v>
+      </c>
+      <c r="F17" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="G17" s="37">
+        <f t="shared" si="3"/>
+        <v>1.9430051813471501</v>
+      </c>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="57"/>
+      <c r="N17">
+        <v>5</v>
+      </c>
+      <c r="O17" s="59">
+        <f>8.5/3.281</f>
+        <v>2.5906735751295336</v>
+      </c>
+      <c r="P17" s="59">
+        <f>0.5/3.281</f>
+        <v>0.15239256324291373</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+      <c r="B18" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="34">
+        <v>1</v>
+      </c>
+      <c r="D18" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E18" s="36">
+        <f t="shared" si="1"/>
+        <v>2.6668698567509903</v>
+      </c>
+      <c r="F18" s="36">
         <f t="shared" si="2"/>
         <v>0.12648582749161841</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G18" s="37">
         <f t="shared" si="3"/>
-        <v>1.9821155725448054</v>
-      </c>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="58"/>
-      <c r="N13">
+        <v>1.6866062032180142</v>
+      </c>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="57"/>
+      <c r="N18">
         <v>5</v>
       </c>
-      <c r="O13" s="82">
-        <f>9.33/3.2/1</f>
-        <v>2.9156249999999999</v>
-      </c>
-      <c r="P13" s="82">
+      <c r="O18" s="59">
+        <f>9/3.281</f>
+        <v>2.7430661383724475</v>
+      </c>
+      <c r="P18" s="59">
         <f>0.33/3.281</f>
         <v>0.10057909174032308</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="35">
+    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+      <c r="B19" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="34">
         <v>1</v>
       </c>
-      <c r="D14" s="37">
+      <c r="D19" s="36">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E14" s="37">
+      <c r="E19" s="36">
         <f t="shared" si="1"/>
-        <v>2.9055418508076807</v>
-      </c>
-      <c r="F14" s="37">
+        <v>2.8447119780554706</v>
+      </c>
+      <c r="F19" s="36">
         <f t="shared" si="2"/>
-        <v>0.12648582749161841</v>
-      </c>
-      <c r="G14" s="38">
+        <v>0.10057909174032308</v>
+      </c>
+      <c r="G19" s="37">
         <f t="shared" si="3"/>
-        <v>1.8375493265546898</v>
-      </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="58"/>
-      <c r="N14">
+        <v>1.4305927350781855</v>
+      </c>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="57"/>
+      <c r="N19">
         <v>5</v>
       </c>
-      <c r="O14" s="82">
+      <c r="O19" s="59">
+        <f>9.667/3.281</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="P19" s="59">
+        <f>0.33/3.281</f>
+        <v>0.10057909174032308</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+      <c r="B20" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="34">
+        <v>1</v>
+      </c>
+      <c r="D20" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E20" s="36">
+        <f t="shared" si="1"/>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="F20" s="36">
+        <f t="shared" si="2"/>
+        <v>0.11429442243218529</v>
+      </c>
+      <c r="G20" s="37">
+        <f t="shared" si="3"/>
+        <v>1.6837613252848753</v>
+      </c>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="57"/>
+      <c r="N20">
+        <v>5</v>
+      </c>
+      <c r="O20" s="59">
+        <f>9.667/3.281</f>
+        <v>2.9463578177384941</v>
+      </c>
+      <c r="P20" s="59">
+        <f>0.42/3.281</f>
+        <v>0.12800975312404753</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="34">
+        <v>1</v>
+      </c>
+      <c r="D21" s="36">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E21" s="36">
+        <f t="shared" si="1"/>
+        <v>3.2256933861627548</v>
+      </c>
+      <c r="F21" s="36">
+        <f t="shared" si="2"/>
+        <v>0.12800975312404753</v>
+      </c>
+      <c r="G21" s="37">
+        <f t="shared" si="3"/>
+        <v>2.0646010700828357</v>
+      </c>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="57"/>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21" s="59">
+        <f>11.5/3.281</f>
+        <v>3.5050289545870159</v>
+      </c>
+      <c r="P21" s="59">
+        <f>0.42/3.281</f>
+        <v>0.12800975312404753</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="34">
+        <v>1</v>
+      </c>
+      <c r="D22" s="36">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E22" s="36">
+        <f t="shared" si="1"/>
+        <v>3.5050289545870159</v>
+      </c>
+      <c r="F22" s="36">
+        <f t="shared" si="2"/>
+        <v>0.14020115818348061</v>
+      </c>
+      <c r="G22" s="37">
+        <f t="shared" si="3"/>
+        <v>2.9484547133984038</v>
+      </c>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="57"/>
+      <c r="N22">
+        <v>6</v>
+      </c>
+      <c r="O22" s="59">
+        <f>11.5/3.281</f>
+        <v>3.5050289545870159</v>
+      </c>
+      <c r="P22" s="59">
+        <f>0.5/3.281</f>
+        <v>0.15239256324291373</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="18"/>
+      <c r="B23" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="34">
+        <v>1</v>
+      </c>
+      <c r="D23" s="36">
+        <f t="shared" ref="D23" si="4">N23</f>
+        <v>8</v>
+      </c>
+      <c r="E23" s="36">
+        <f t="shared" si="1"/>
+        <v>3.2002438281011885</v>
+      </c>
+      <c r="F23" s="36">
+        <f t="shared" si="2"/>
+        <v>0.15119628162145687</v>
+      </c>
+      <c r="G23" s="37">
+        <f t="shared" ref="G23" si="5">PRODUCT(C23:F23)</f>
+        <v>3.8709197367273322</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="57"/>
+      <c r="N23">
+        <v>8</v>
+      </c>
+      <c r="O23" s="59">
         <f>9.5/3.281</f>
         <v>2.895458701615361</v>
       </c>
-      <c r="P14" s="82">
-        <f>0.5/3.281</f>
-        <v>0.15239256324291373</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="35">
-        <v>1</v>
-      </c>
-      <c r="D15" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E15" s="37">
-        <f t="shared" si="1"/>
-        <v>2.8192624199939043</v>
-      </c>
-      <c r="F15" s="37">
-        <v>0.15</v>
-      </c>
-      <c r="G15" s="38">
-        <f t="shared" si="3"/>
-        <v>2.1144468149954281</v>
-      </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="58"/>
-      <c r="N15">
-        <v>5</v>
-      </c>
-      <c r="O15" s="82">
-        <f>9/3.281</f>
-        <v>2.7430661383724475</v>
-      </c>
-      <c r="P15" s="82">
-        <f>0.583/3.281</f>
-        <v>0.1776897287412374</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="C16" s="35">
-        <v>1</v>
-      </c>
-      <c r="D16" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E16" s="37">
-        <f t="shared" si="1"/>
-        <v>2.6668698567509903</v>
-      </c>
-      <c r="F16" s="37">
-        <v>0.15</v>
-      </c>
-      <c r="G16" s="38">
-        <f t="shared" si="3"/>
-        <v>2.0001523925632427</v>
-      </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="58"/>
-      <c r="N16">
-        <v>5</v>
-      </c>
-      <c r="O16" s="82">
-        <f>8.5/3.281</f>
-        <v>2.5906735751295336</v>
-      </c>
-      <c r="P16" s="82">
-        <f>0.75/3.281</f>
-        <v>0.22858884486437062</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="35">
-        <v>1</v>
-      </c>
-      <c r="D17" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E17" s="37">
-        <f t="shared" si="1"/>
-        <v>2.5906735751295336</v>
-      </c>
-      <c r="F17" s="37">
-        <v>0.15</v>
-      </c>
-      <c r="G17" s="38">
-        <f t="shared" si="3"/>
-        <v>1.9430051813471501</v>
-      </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="58"/>
-      <c r="N17">
-        <v>5</v>
-      </c>
-      <c r="O17" s="82">
-        <f>8.5/3.281</f>
-        <v>2.5906735751295336</v>
-      </c>
-      <c r="P17" s="82">
-        <f>0.5/3.281</f>
-        <v>0.15239256324291373</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="35">
-        <v>1</v>
-      </c>
-      <c r="D18" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E18" s="37">
-        <f t="shared" si="1"/>
-        <v>2.6668698567509903</v>
-      </c>
-      <c r="F18" s="37">
-        <f t="shared" si="2"/>
-        <v>0.12648582749161841</v>
-      </c>
-      <c r="G18" s="38">
-        <f t="shared" si="3"/>
-        <v>1.6866062032180142</v>
-      </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="58"/>
-      <c r="N18">
-        <v>5</v>
-      </c>
-      <c r="O18" s="82">
-        <f>9/3.281</f>
-        <v>2.7430661383724475</v>
-      </c>
-      <c r="P18" s="82">
-        <f>0.33/3.281</f>
-        <v>0.10057909174032308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="35">
-        <v>1</v>
-      </c>
-      <c r="D19" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E19" s="37">
-        <f t="shared" si="1"/>
-        <v>2.8447119780554706</v>
-      </c>
-      <c r="F19" s="37">
-        <f t="shared" si="2"/>
-        <v>0.10057909174032308</v>
-      </c>
-      <c r="G19" s="38">
-        <f t="shared" si="3"/>
-        <v>1.4305927350781855</v>
-      </c>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="58"/>
-      <c r="N19">
-        <v>5</v>
-      </c>
-      <c r="O19" s="82">
-        <f>9.667/3.281</f>
-        <v>2.9463578177384941</v>
-      </c>
-      <c r="P19" s="82">
-        <f>0.33/3.281</f>
-        <v>0.10057909174032308</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="C20" s="35">
-        <v>1</v>
-      </c>
-      <c r="D20" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E20" s="37">
-        <f t="shared" si="1"/>
-        <v>2.9463578177384941</v>
-      </c>
-      <c r="F20" s="37">
-        <f t="shared" si="2"/>
-        <v>0.11429442243218529</v>
-      </c>
-      <c r="G20" s="38">
-        <f t="shared" si="3"/>
-        <v>1.6837613252848753</v>
-      </c>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="58"/>
-      <c r="N20">
-        <v>5</v>
-      </c>
-      <c r="O20" s="82">
-        <f>9.667/3.281</f>
-        <v>2.9463578177384941</v>
-      </c>
-      <c r="P20" s="82">
-        <f>0.42/3.281</f>
-        <v>0.12800975312404753</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="35">
-        <v>1</v>
-      </c>
-      <c r="D21" s="37">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E21" s="37">
-        <f t="shared" si="1"/>
-        <v>3.2135019811033221</v>
-      </c>
-      <c r="F21" s="37">
-        <f t="shared" si="2"/>
-        <v>0.12800975312404753</v>
-      </c>
-      <c r="G21" s="38">
-        <f t="shared" si="3"/>
-        <v>2.0567979763233692</v>
-      </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="58"/>
-      <c r="N21">
-        <v>5</v>
-      </c>
-      <c r="O21" s="82">
-        <f>11.42/3.281</f>
-        <v>3.4806461444681496</v>
-      </c>
-      <c r="P21" s="82">
-        <f>0.42/3.281</f>
-        <v>0.12800975312404753</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C22" s="35">
-        <v>1</v>
-      </c>
-      <c r="D22" s="37">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E22" s="37">
-        <f t="shared" si="1"/>
-        <v>3.4806461444681496</v>
-      </c>
-      <c r="F22" s="37">
-        <f t="shared" si="2"/>
-        <v>0.14020115818348061</v>
-      </c>
-      <c r="G22" s="38">
-        <f t="shared" si="3"/>
-        <v>2.9279437240878057</v>
-      </c>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="58"/>
-      <c r="N22">
-        <v>6</v>
-      </c>
-      <c r="O22" s="82">
-        <f>11.42/3.281</f>
-        <v>3.4806461444681496</v>
-      </c>
-      <c r="P22" s="82">
-        <f>0.5/3.281</f>
-        <v>0.15239256324291373</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="35">
-        <v>1</v>
-      </c>
-      <c r="D23" s="37">
-        <f t="shared" ref="D23" si="4">N23</f>
-        <v>8</v>
-      </c>
-      <c r="E23" s="37">
-        <f t="shared" si="1"/>
-        <v>3.1880524230417553</v>
-      </c>
-      <c r="F23" s="37">
-        <f t="shared" si="2"/>
-        <v>0.15119628162145687</v>
-      </c>
-      <c r="G23" s="38">
-        <f t="shared" ref="G23" si="5">PRODUCT(C23:F23)</f>
-        <v>3.8561733758255134</v>
-      </c>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="58"/>
-      <c r="N23">
-        <v>8</v>
-      </c>
-      <c r="O23" s="82">
-        <f>9.5/3.281</f>
-        <v>2.895458701615361</v>
-      </c>
-      <c r="P23" s="82">
+      <c r="P23" s="59">
         <v>0.15</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>41</v>
       </c>
       <c r="C24" s="19"/>
@@ -3058,7 +3058,7 @@
       <c r="F24" s="21"/>
       <c r="G24" s="23">
         <f>SUM(G11:G23)</f>
-        <v>27.387017442225286</v>
+        <v>27.844258417424825</v>
       </c>
       <c r="H24" s="22" t="s">
         <v>40</v>
@@ -3066,15 +3066,15 @@
       <c r="I24" s="23">
         <v>1693.85</v>
       </c>
-      <c r="J24" s="40">
+      <c r="J24" s="39">
         <f>G24*I24</f>
-        <v>46389.4994945133</v>
-      </c>
-      <c r="K24" s="58"/>
+        <v>47163.997120355038</v>
+      </c>
+      <c r="K24" s="57"/>
     </row>
     <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="19"/>
@@ -3084,9 +3084,9 @@
       <c r="G25" s="23"/>
       <c r="H25" s="22"/>
       <c r="I25" s="23"/>
-      <c r="J25" s="40">
+      <c r="J25" s="39">
         <f>0.13*G24*446551.8/300</f>
-        <v>5299.5461720314088</v>
+        <v>5388.0249435853566</v>
       </c>
       <c r="K25" s="21"/>
     </row>
@@ -3100,7 +3100,7 @@
       <c r="G26" s="23"/>
       <c r="H26" s="22"/>
       <c r="I26" s="23"/>
-      <c r="J26" s="40"/>
+      <c r="J26" s="39"/>
       <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3111,14 +3111,14 @@
         <v>30</v>
       </c>
       <c r="C27" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" s="20"/>
       <c r="E27" s="21"/>
       <c r="F27" s="21"/>
-      <c r="G27" s="33">
+      <c r="G27" s="32">
         <f t="shared" ref="G27" si="6">PRODUCT(C27:F27)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H27" s="22" t="s">
         <v>31</v>
@@ -3126,9 +3126,9 @@
       <c r="I27" s="23">
         <v>500</v>
       </c>
-      <c r="J27" s="33">
+      <c r="J27" s="32">
         <f>G27*I27</f>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="K27" s="21"/>
     </row>
@@ -3142,230 +3142,237 @@
       <c r="G28" s="23"/>
       <c r="H28" s="22"/>
       <c r="I28" s="23"/>
-      <c r="J28" s="40"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="21"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" s="39"/>
-      <c r="B29" s="41" t="s">
+      <c r="A29" s="38"/>
+      <c r="B29" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40">
+      <c r="C29" s="41"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39">
         <f>SUM(J9:J27)</f>
-        <v>52189.045666544713</v>
-      </c>
-      <c r="K29" s="35"/>
+        <v>52552.022063940392</v>
+      </c>
+      <c r="K29" s="34"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="53"/>
-      <c r="B30" s="56"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="54"/>
-      <c r="E30" s="54"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="55"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="52"/>
+      <c r="A30" s="52"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="51"/>
     </row>
     <row r="31" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="45"/>
+      <c r="A31" s="44"/>
       <c r="B31" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="60">
+      <c r="C31" s="61">
         <f>J29</f>
-        <v>52189.045666544713</v>
-      </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="38">
+        <v>52552.022063940392</v>
+      </c>
+      <c r="D31" s="61"/>
+      <c r="E31" s="37">
         <v>100</v>
       </c>
-      <c r="F31" s="46"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="46"/>
-      <c r="I31" s="48"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="50"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="49"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="51"/>
+      <c r="A32" s="50"/>
       <c r="B32" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="81">
+      <c r="C32" s="62">
         <v>50000</v>
       </c>
-      <c r="D32" s="81"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
-      <c r="K32" s="44"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="43"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="51"/>
+      <c r="A33" s="50"/>
       <c r="B33" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C33" s="81">
+      <c r="C33" s="62">
         <f>C32-C35-C36</f>
         <v>47500</v>
       </c>
-      <c r="D33" s="81"/>
-      <c r="E33" s="38">
+      <c r="D33" s="62"/>
+      <c r="E33" s="37">
         <f>C33/C31*100</f>
-        <v>91.015268421452319</v>
-      </c>
-      <c r="F33" s="44"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
-      <c r="K33" s="44"/>
+        <v>90.386626688134726</v>
+      </c>
+      <c r="F33" s="43"/>
+      <c r="G33" s="42"/>
+      <c r="H33" s="42"/>
+      <c r="I33" s="42"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="43"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="51"/>
+      <c r="A34" s="50"/>
       <c r="B34" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="C34" s="60">
+      <c r="C34" s="61">
         <f>C31-C33</f>
-        <v>4689.0456665447127</v>
-      </c>
-      <c r="D34" s="60"/>
-      <c r="E34" s="38">
+        <v>5052.0220639403924</v>
+      </c>
+      <c r="D34" s="61"/>
+      <c r="E34" s="37">
         <f>100-E33</f>
-        <v>8.9847315785476809</v>
-      </c>
-      <c r="F34" s="44"/>
-      <c r="G34" s="43"/>
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
-      <c r="K34" s="44"/>
+        <v>9.6133733118652742</v>
+      </c>
+      <c r="F34" s="43"/>
+      <c r="G34" s="42"/>
+      <c r="H34" s="42"/>
+      <c r="I34" s="42"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="43"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="51"/>
+      <c r="A35" s="50"/>
       <c r="B35" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="60">
+      <c r="C35" s="61">
         <f>C32*0.03</f>
         <v>1500</v>
       </c>
-      <c r="D35" s="60"/>
-      <c r="E35" s="38">
+      <c r="D35" s="61"/>
+      <c r="E35" s="37">
         <v>3</v>
       </c>
-      <c r="F35" s="44"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="44"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="43"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="51"/>
+      <c r="A36" s="50"/>
       <c r="B36" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C36" s="60">
+      <c r="C36" s="61">
         <f>C32*0.02</f>
         <v>1000</v>
       </c>
-      <c r="D36" s="60"/>
-      <c r="E36" s="38">
+      <c r="D36" s="61"/>
+      <c r="E36" s="37">
         <v>2</v>
       </c>
-      <c r="F36" s="44"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
-      <c r="K36" s="44"/>
-    </row>
-    <row r="37" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="52"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="52"/>
-    </row>
-    <row r="38" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="34" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="43"/>
+    </row>
+    <row r="37" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="51"/>
+      <c r="B37" s="51"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="51"/>
+      <c r="K37" s="51"/>
+    </row>
+    <row r="38" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:11" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="54" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="58" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="60" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="61" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="63" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="65" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="66" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="81" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="82" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="83" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="84" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="86" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="87" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="88" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="89" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="90" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="91" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C35:D35"/>
     <mergeCell ref="C36:D36"/>
     <mergeCell ref="A7:F7"/>
@@ -3374,13 +3381,6 @@
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C33:D33"/>
     <mergeCell ref="C34:D34"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:F6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>